<commit_message>
Display functions updated + refactoring
</commit_message>
<xml_diff>
--- a/arguments_overview.xlsx
+++ b/arguments_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshmc\Documents\UAB\+ TA Stuff\Trello_C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9C32E3-45B1-4357-9A54-1500721D5990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4363447-DBE7-41DA-99A7-5FFF61180171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="22275" windowHeight="14070" xr2:uid="{7AF23832-23D9-45D1-8EA2-26E6DEEFBC19}"/>
+    <workbookView xWindow="31785" yWindow="555" windowWidth="22275" windowHeight="14070" xr2:uid="{7AF23832-23D9-45D1-8EA2-26E6DEEFBC19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>trello.exe</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>/priority</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -516,19 +522,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78F1DA1-976F-48B3-BBE1-0E73AF8052AB}">
-  <dimension ref="B3:G26"/>
+  <dimension ref="B2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -548,7 +563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -568,7 +583,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -576,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -584,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -598,7 +613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -612,7 +627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -626,7 +641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -640,7 +655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -657,7 +672,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -671,7 +686,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -688,7 +703,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -699,7 +714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -710,7 +725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>

</xml_diff>